<commit_message>
Added test data for Search Transactions
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Misc-Data.xlsx
+++ b/Bootstrap/VT-Misc-Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F943763-AFF3-4ACD-8335-3EE0413121B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19CD59B-0A80-45AA-BDB9-8320E63E33CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="3" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView xWindow="3405" yWindow="3150" windowWidth="21600" windowHeight="12735" activeTab="4" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
     <sheet name="Capture-MoreError" sheetId="2" r:id="rId2"/>
     <sheet name="FieldValidationError" sheetId="6" r:id="rId3"/>
     <sheet name="SearchTransactions" sheetId="7" r:id="rId4"/>
+    <sheet name="SaleSearchTransactions" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="138">
   <si>
     <t>Result</t>
   </si>
@@ -353,6 +354,105 @@
   </si>
   <si>
     <t>Text Receipt Phone Number is invalid</t>
+  </si>
+  <si>
+    <t>6011000993026909</t>
+  </si>
+  <si>
+    <t>Discover</t>
+  </si>
+  <si>
+    <t>6909</t>
+  </si>
+  <si>
+    <t>Mithun Chakravarthy</t>
+  </si>
+  <si>
+    <t>6565 Jhilmil Palace</t>
+  </si>
+  <si>
+    <t>21093</t>
+  </si>
+  <si>
+    <t>Yaad aa raha hai</t>
+  </si>
+  <si>
+    <t>Tera Pyar</t>
+  </si>
+  <si>
+    <t>Yaron Main to</t>
+  </si>
+  <si>
+    <t>Yahan Jeeta raha</t>
+  </si>
+  <si>
+    <t>Saare Ghum</t>
+  </si>
+  <si>
+    <t>Apne Bhula ke</t>
+  </si>
+  <si>
+    <t>MITHUN CHAKRAVARTHY</t>
+  </si>
+  <si>
+    <t>SearchBy</t>
+  </si>
+  <si>
+    <t>Remittance ID</t>
+  </si>
+  <si>
+    <t>Payment ID</t>
+  </si>
+  <si>
+    <t>CC last 4 digit</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Payer Name</t>
+  </si>
+  <si>
+    <t>Client Account Number</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF1</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF2</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF3</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF4</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF5</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF6</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF7</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF8</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF9</t>
+  </si>
+  <si>
+    <t>UDF Label: UDF 10</t>
+  </si>
+  <si>
+    <t>mithunda79@gmail.com</t>
+  </si>
+  <si>
+    <t>SearchValue</t>
+  </si>
+  <si>
+    <t>17.50</t>
   </si>
 </sst>
 </file>
@@ -409,13 +509,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2434,7 +2535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A29DF0-E80A-4D1A-9523-089EBE8AD58D}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -2515,4 +2616,1921 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
+  <dimension ref="A1:AK19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="10.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="3" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="28.140625" style="3" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="25" style="3" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="3"/>
+    <col min="23" max="23" width="17.7109375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="16" style="3" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="18.85546875" style="3" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" style="3" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="22" style="3" customWidth="1"/>
+    <col min="31" max="31" width="24.42578125" style="3" customWidth="1"/>
+    <col min="32" max="32" width="21.85546875" style="3" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" style="3" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" style="3"/>
+    <col min="35" max="35" width="30.42578125" style="3" customWidth="1"/>
+    <col min="36" max="36" width="25.28515625" style="3" customWidth="1"/>
+    <col min="37" max="37" width="26" style="3" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test data for ACH
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Misc-Data.xlsx
+++ b/Bootstrap/VT-Misc-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19CD59B-0A80-45AA-BDB9-8320E63E33CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45BC725-2195-4DB1-8878-058CD1467734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="3150" windowWidth="21600" windowHeight="12735" activeTab="4" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="139">
   <si>
     <t>Result</t>
   </si>
@@ -413,9 +413,6 @@
     <t>Payer Name</t>
   </si>
   <si>
-    <t>Client Account Number</t>
-  </si>
-  <si>
     <t>UDF Label: UDF1</t>
   </si>
   <si>
@@ -453,6 +450,12 @@
   </si>
   <si>
     <t>17.50</t>
+  </si>
+  <si>
+    <t>Orange Recorded</t>
+  </si>
+  <si>
+    <t>Yellow Recorded</t>
   </si>
 </sst>
 </file>
@@ -2620,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
-  <dimension ref="A1:AK19"/>
+  <dimension ref="A1:AK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AD9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,13 +2774,10 @@
         <v>118</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
@@ -2870,9 +2870,6 @@
       </c>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="1" t="s">
         <v>70</v>
       </c>
@@ -2965,9 +2962,6 @@
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E4" s="1" t="s">
         <v>70</v>
       </c>
@@ -3063,9 +3057,6 @@
       </c>
     </row>
     <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3112,7 +3103,7 @@
         <v>110</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>41</v>
@@ -3160,13 +3151,10 @@
         <v>122</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" s="1" t="s">
         <v>70</v>
       </c>
@@ -3213,7 +3201,7 @@
         <v>110</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>111</v>
@@ -3258,13 +3246,10 @@
         <v>17</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="1" t="s">
         <v>70</v>
       </c>
@@ -3360,9 +3345,6 @@
       </c>
     </row>
     <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="1" t="s">
         <v>70</v>
       </c>
@@ -3483,7 +3465,7 @@
         <v>56</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>35</v>
@@ -3537,10 +3519,10 @@
         <v>112</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="AI9" s="1" t="s">
         <v>117</v>
@@ -3548,11 +3530,11 @@
       <c r="AJ9" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="AK9" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>70</v>
       </c>
@@ -3644,13 +3626,10 @@
         <v>125</v>
       </c>
       <c r="AK10" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E11" s="1" t="s">
         <v>70</v>
       </c>
@@ -3742,13 +3721,10 @@
         <v>126</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" s="1" t="s">
         <v>70</v>
       </c>
@@ -3840,7 +3816,7 @@
         <v>127</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3938,13 +3914,10 @@
         <v>128</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E14" s="1" t="s">
         <v>70</v>
       </c>
@@ -4036,13 +4009,10 @@
         <v>129</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E15" s="1" t="s">
         <v>70</v>
       </c>
@@ -4134,13 +4104,10 @@
         <v>130</v>
       </c>
       <c r="AK15" s="1" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E16" s="1" t="s">
         <v>70</v>
       </c>
@@ -4232,13 +4199,10 @@
         <v>131</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="17" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
+    <row r="17" spans="5:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>70</v>
       </c>
@@ -4330,13 +4294,10 @@
         <v>132</v>
       </c>
       <c r="AK17" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="18" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
-        <v>31</v>
-      </c>
+    <row r="18" spans="5:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>70</v>
       </c>
@@ -4428,104 +4389,6 @@
         <v>133</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="X19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI19" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK19" s="1" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test data for card not accepted
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Misc-Data.xlsx
+++ b/Bootstrap/VT-Misc-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC6B0FD-6251-49D1-9283-1D92348F3BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF221B95-4B17-4798-9D94-B071A6789AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="4530" windowWidth="21600" windowHeight="12735" firstSheet="3" activeTab="7" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="8" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="ConfirmAcNumError" sheetId="9" r:id="rId6"/>
     <sheet name="Debit-CAN" sheetId="10" r:id="rId7"/>
     <sheet name="Sale-CAN" sheetId="11" r:id="rId8"/>
+    <sheet name="Sale-CardNotAccepted" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="173">
   <si>
     <t>Result</t>
   </si>
@@ -558,6 +559,9 @@
   </si>
   <si>
     <t>14.50</t>
+  </si>
+  <si>
+    <t>Card Notaccepted</t>
   </si>
 </sst>
 </file>
@@ -5045,8 +5049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58603BCF-4622-4E65-9487-561DE995DE00}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5287,4 +5291,258 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
+  <dimension ref="A1:AB3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.140625" style="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" style="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>